<commit_message>
Added moments of inertia, etc... to excel file
</commit_message>
<xml_diff>
--- a/Quadcopter.xlsx
+++ b/Quadcopter.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\Quadcopter-Demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -220,6 +225,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -236,10 +309,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="141414"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F8F8F8"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -486,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>